<commit_message>
implement export-to-excels and controllers
</commit_message>
<xml_diff>
--- a/src/main/resources/static/customer.xlsx
+++ b/src/main/resources/static/customer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\parsparand-reporter-application\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\parsparand-reporter-application\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C14121-9836-4E30-8436-A07C2C90473E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42574965-2F97-42D6-9592-31D9CDAD92F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="827">
   <si>
     <t>id</t>
   </si>
@@ -2410,6 +2410,99 @@
   </si>
   <si>
     <t>nationalCode</t>
+  </si>
+  <si>
+    <t>آنیل شیمی سپاهان</t>
+  </si>
+  <si>
+    <t>صنایع غذایی رضوی</t>
+  </si>
+  <si>
+    <t>پترو آکام راد صنعت</t>
+  </si>
+  <si>
+    <t>جاوید بنیان هیواد</t>
+  </si>
+  <si>
+    <t>آویسا پارسه زابل</t>
+  </si>
+  <si>
+    <t>پژوهشکده صنعت نفت</t>
+  </si>
+  <si>
+    <t>محمد مهدی رضائی(راننده)</t>
+  </si>
+  <si>
+    <t>بهیین تامین اهورا</t>
+  </si>
+  <si>
+    <t>سیدمهدی موسوی</t>
+  </si>
+  <si>
+    <t>سجاد علی اکبری</t>
+  </si>
+  <si>
+    <t>سیدحسین موسوی</t>
+  </si>
+  <si>
+    <t>مهندسی موادکاران جاهد نوآور</t>
+  </si>
+  <si>
+    <t>مسعود علی پور</t>
+  </si>
+  <si>
+    <t>احسان شیمی استهبان</t>
+  </si>
+  <si>
+    <t>پالایش نفت و گاز پیروزی</t>
+  </si>
+  <si>
+    <t>محمدحسین گرامی</t>
+  </si>
+  <si>
+    <t>پالایش نفت بندرعباس</t>
+  </si>
+  <si>
+    <t>صنایع شیمیایی ریف ایران</t>
+  </si>
+  <si>
+    <t>حسن قرقانی</t>
+  </si>
+  <si>
+    <t>کیمیا گران امروز</t>
+  </si>
+  <si>
+    <t>امیر صنعت نقش آذین</t>
+  </si>
+  <si>
+    <t>نفت و گاز سرو</t>
+  </si>
+  <si>
+    <t>بازرگانی چاپار افرند</t>
+  </si>
+  <si>
+    <t>احمد جهانشاهی</t>
+  </si>
+  <si>
+    <t>تکوین آرمه</t>
+  </si>
+  <si>
+    <t>مرتضی مظاهری</t>
+  </si>
+  <si>
+    <t>رضا هونجانی</t>
+  </si>
+  <si>
+    <t>شیمی پالایش البرز غرب</t>
+  </si>
+  <si>
+    <t>محمدرضا ناورانی</t>
+  </si>
+  <si>
+    <t>روغن موتور تکتازتوان بی نظیر</t>
+  </si>
+  <si>
+    <t>فردین کاویانی دره شوری</t>
   </si>
 </sst>
 </file>
@@ -2926,10 +3019,21 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3285,17 +3389,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G240"/>
+  <dimension ref="A1:G276"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -3303,36 +3407,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>792</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>793</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>794</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>795</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="5">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -3349,13 +3453,13 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="5">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -3372,13 +3476,13 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="5">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -3395,13 +3499,13 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="5">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -3418,13 +3522,13 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="5">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -3441,13 +3545,13 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="5">
         <v>0</v>
       </c>
       <c r="B7" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -3464,13 +3568,13 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="5">
         <v>0</v>
       </c>
       <c r="B8" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -3487,13 +3591,13 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="5">
         <v>0</v>
       </c>
       <c r="B9" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -3510,13 +3614,13 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="5">
         <v>0</v>
       </c>
       <c r="B10" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -3533,13 +3637,13 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="5">
         <v>0</v>
       </c>
       <c r="B11" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -3556,13 +3660,13 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="5">
         <v>0</v>
       </c>
       <c r="B12" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -3579,13 +3683,13 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="5">
         <v>0</v>
       </c>
       <c r="B13" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -3602,13 +3706,13 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="5">
         <v>0</v>
       </c>
       <c r="B14" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -3625,13 +3729,13 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="5">
         <v>0</v>
       </c>
       <c r="B15" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -3648,13 +3752,13 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="5">
         <v>0</v>
       </c>
       <c r="B16" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -3671,13 +3775,13 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="5">
         <v>0</v>
       </c>
       <c r="B17" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -3694,13 +3798,13 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="5">
         <v>0</v>
       </c>
       <c r="B18" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -3717,13 +3821,13 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="5">
         <v>0</v>
       </c>
       <c r="B19" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="3" t="s">
         <v>60</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -3740,13 +3844,13 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="A20" s="5">
         <v>0</v>
       </c>
       <c r="B20" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -3763,13 +3867,13 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="5">
         <v>0</v>
       </c>
       <c r="B21" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -3786,13 +3890,13 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="5">
         <v>0</v>
       </c>
       <c r="B22" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -3809,13 +3913,13 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="5">
         <v>0</v>
       </c>
       <c r="B23" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -3832,13 +3936,13 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="A24" s="5">
         <v>0</v>
       </c>
       <c r="B24" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="3" t="s">
         <v>75</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -3855,13 +3959,13 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="A25" s="5">
         <v>0</v>
       </c>
       <c r="B25" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="3" t="s">
         <v>78</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -3878,13 +3982,13 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="A26" s="5">
         <v>0</v>
       </c>
       <c r="B26" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="3" t="s">
         <v>81</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -3901,13 +4005,13 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="A27" s="5">
         <v>0</v>
       </c>
       <c r="B27" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="3" t="s">
         <v>84</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -3924,13 +4028,13 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="A28" s="5">
         <v>0</v>
       </c>
       <c r="B28" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="3" t="s">
         <v>87</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -3947,13 +4051,13 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="A29" s="5">
         <v>0</v>
       </c>
       <c r="B29" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="3" t="s">
         <v>90</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -3970,13 +4074,13 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="A30" s="5">
         <v>0</v>
       </c>
       <c r="B30" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="3" t="s">
         <v>94</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -3993,13 +4097,13 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="A31" s="5">
         <v>0</v>
       </c>
       <c r="B31" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -4016,13 +4120,13 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="A32" s="5">
         <v>0</v>
       </c>
       <c r="B32" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="3" t="s">
         <v>102</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -4039,13 +4143,13 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="A33" s="5">
         <v>0</v>
       </c>
       <c r="B33" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="3" t="s">
         <v>106</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -4062,13 +4166,13 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="A34" s="5">
         <v>0</v>
       </c>
       <c r="B34" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="3" t="s">
         <v>110</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -4085,13 +4189,13 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="A35" s="5">
         <v>0</v>
       </c>
       <c r="B35" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="3" t="s">
         <v>113</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -4108,13 +4212,13 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="A36" s="5">
         <v>0</v>
       </c>
       <c r="B36" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -4131,13 +4235,13 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+      <c r="A37" s="5">
         <v>0</v>
       </c>
       <c r="B37" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="3" t="s">
         <v>119</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -4154,13 +4258,13 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+      <c r="A38" s="5">
         <v>0</v>
       </c>
       <c r="B38" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="3" t="s">
         <v>122</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -4177,13 +4281,13 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
+      <c r="A39" s="5">
         <v>0</v>
       </c>
       <c r="B39" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="3" t="s">
         <v>125</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -4200,13 +4304,13 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
+      <c r="A40" s="5">
         <v>0</v>
       </c>
       <c r="B40" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="3" t="s">
         <v>129</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -4223,13 +4327,13 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+      <c r="A41" s="5">
         <v>0</v>
       </c>
       <c r="B41" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="3" t="s">
         <v>132</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -4246,13 +4350,13 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+      <c r="A42" s="5">
         <v>0</v>
       </c>
       <c r="B42" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="3" t="s">
         <v>135</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -4269,13 +4373,13 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+      <c r="A43" s="5">
         <v>0</v>
       </c>
       <c r="B43" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="3" t="s">
         <v>138</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -4292,13 +4396,13 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+      <c r="A44" s="5">
         <v>0</v>
       </c>
       <c r="B44" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="3" t="s">
         <v>141</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -4315,13 +4419,13 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
+      <c r="A45" s="5">
         <v>0</v>
       </c>
       <c r="B45" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -4338,13 +4442,13 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+      <c r="A46" s="5">
         <v>0</v>
       </c>
       <c r="B46" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="3" t="s">
         <v>148</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -4361,13 +4465,13 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+      <c r="A47" s="5">
         <v>0</v>
       </c>
       <c r="B47" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="3" t="s">
         <v>152</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -4384,13 +4488,13 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+      <c r="A48" s="5">
         <v>0</v>
       </c>
       <c r="B48" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="3" t="s">
         <v>155</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -4407,13 +4511,13 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
+      <c r="A49" s="5">
         <v>0</v>
       </c>
       <c r="B49" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="3" t="s">
         <v>158</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -4430,13 +4534,13 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
+      <c r="A50" s="5">
         <v>0</v>
       </c>
       <c r="B50" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="3" t="s">
         <v>162</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -4453,13 +4557,13 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
+      <c r="A51" s="5">
         <v>0</v>
       </c>
       <c r="B51" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="3" t="s">
         <v>166</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -4476,13 +4580,13 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
+      <c r="A52" s="5">
         <v>0</v>
       </c>
       <c r="B52" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="3" t="s">
         <v>169</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -4499,13 +4603,13 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
+      <c r="A53" s="5">
         <v>0</v>
       </c>
       <c r="B53" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="3" t="s">
         <v>172</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -4522,13 +4626,13 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
+      <c r="A54" s="5">
         <v>0</v>
       </c>
       <c r="B54" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="3" t="s">
         <v>175</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -4545,13 +4649,13 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
+      <c r="A55" s="5">
         <v>0</v>
       </c>
       <c r="B55" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="3" t="s">
         <v>178</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -4568,13 +4672,13 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
+      <c r="A56" s="5">
         <v>0</v>
       </c>
       <c r="B56" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="3" t="s">
         <v>181</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -4591,13 +4695,13 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
+      <c r="A57" s="5">
         <v>0</v>
       </c>
       <c r="B57" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="3" t="s">
         <v>184</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -4614,13 +4718,13 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
+      <c r="A58" s="5">
         <v>0</v>
       </c>
       <c r="B58" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="3" t="s">
         <v>188</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -4637,13 +4741,13 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
+      <c r="A59" s="5">
         <v>0</v>
       </c>
       <c r="B59" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="3" t="s">
         <v>191</v>
       </c>
       <c r="D59" s="1" t="s">
@@ -4660,13 +4764,13 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
+      <c r="A60" s="5">
         <v>0</v>
       </c>
       <c r="B60" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="3" t="s">
         <v>195</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -4683,13 +4787,13 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
+      <c r="A61" s="5">
         <v>0</v>
       </c>
       <c r="B61" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="3" t="s">
         <v>198</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -4706,13 +4810,13 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
+      <c r="A62" s="5">
         <v>0</v>
       </c>
       <c r="B62" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="3" t="s">
         <v>201</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -4729,13 +4833,13 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
+      <c r="A63" s="5">
         <v>0</v>
       </c>
       <c r="B63" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="3" t="s">
         <v>204</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -4752,13 +4856,13 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
+      <c r="A64" s="5">
         <v>0</v>
       </c>
       <c r="B64" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -4775,13 +4879,13 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
+      <c r="A65" s="5">
         <v>0</v>
       </c>
       <c r="B65" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="3" t="s">
         <v>211</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -4798,13 +4902,13 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
+      <c r="A66" s="5">
         <v>0</v>
       </c>
       <c r="B66" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="3" t="s">
         <v>215</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -4821,13 +4925,13 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
+      <c r="A67" s="5">
         <v>0</v>
       </c>
       <c r="B67" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="3" t="s">
         <v>218</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -4844,13 +4948,13 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
+      <c r="A68" s="5">
         <v>0</v>
       </c>
       <c r="B68" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="3" t="s">
         <v>221</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -4867,13 +4971,13 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
+      <c r="A69" s="5">
         <v>0</v>
       </c>
       <c r="B69" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" s="3" t="s">
         <v>224</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -4890,13 +4994,13 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
+      <c r="A70" s="5">
         <v>0</v>
       </c>
       <c r="B70" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="3" t="s">
         <v>227</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -4913,13 +5017,13 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="2">
+      <c r="A71" s="5">
         <v>0</v>
       </c>
       <c r="B71" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="3" t="s">
         <v>230</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -4936,13 +5040,13 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="2">
+      <c r="A72" s="5">
         <v>0</v>
       </c>
       <c r="B72" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="3" t="s">
         <v>233</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -4959,13 +5063,13 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="2">
+      <c r="A73" s="5">
         <v>0</v>
       </c>
       <c r="B73" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="3" t="s">
         <v>236</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -4982,13 +5086,13 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="2">
+      <c r="A74" s="5">
         <v>0</v>
       </c>
       <c r="B74" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="3" t="s">
         <v>239</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -5005,13 +5109,13 @@
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="2">
+      <c r="A75" s="5">
         <v>0</v>
       </c>
       <c r="B75" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" s="3" t="s">
         <v>242</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -5028,13 +5132,13 @@
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="2">
+      <c r="A76" s="5">
         <v>0</v>
       </c>
       <c r="B76" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="3" t="s">
         <v>245</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -5051,13 +5155,13 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
+      <c r="A77" s="5">
         <v>0</v>
       </c>
       <c r="B77" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="3" t="s">
         <v>248</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -5074,13 +5178,13 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="2">
+      <c r="A78" s="5">
         <v>0</v>
       </c>
       <c r="B78" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="3" t="s">
         <v>251</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -5097,13 +5201,13 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="2">
+      <c r="A79" s="5">
         <v>0</v>
       </c>
       <c r="B79" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" s="3" t="s">
         <v>254</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -5120,13 +5224,13 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
+      <c r="A80" s="5">
         <v>0</v>
       </c>
       <c r="B80" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="3" t="s">
         <v>257</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -5143,13 +5247,13 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
+      <c r="A81" s="5">
         <v>0</v>
       </c>
       <c r="B81" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" s="3" t="s">
         <v>260</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -5166,13 +5270,13 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
+      <c r="A82" s="5">
         <v>0</v>
       </c>
       <c r="B82" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" s="3" t="s">
         <v>263</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -5189,13 +5293,13 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="2">
+      <c r="A83" s="5">
         <v>0</v>
       </c>
       <c r="B83" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" s="3" t="s">
         <v>266</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -5212,13 +5316,13 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
+      <c r="A84" s="5">
         <v>0</v>
       </c>
       <c r="B84" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" s="3" t="s">
         <v>270</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -5235,13 +5339,13 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="2">
+      <c r="A85" s="5">
         <v>0</v>
       </c>
       <c r="B85" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" s="3" t="s">
         <v>273</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -5258,13 +5362,13 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="2">
+      <c r="A86" s="5">
         <v>0</v>
       </c>
       <c r="B86" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" s="3" t="s">
         <v>276</v>
       </c>
       <c r="D86" s="1" t="s">
@@ -5281,13 +5385,13 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
+      <c r="A87" s="5">
         <v>0</v>
       </c>
       <c r="B87" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" s="3" t="s">
         <v>278</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -5304,13 +5408,13 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="2">
+      <c r="A88" s="5">
         <v>0</v>
       </c>
       <c r="B88" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" s="3" t="s">
         <v>282</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -5327,13 +5431,13 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="2">
+      <c r="A89" s="5">
         <v>0</v>
       </c>
       <c r="B89" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" s="3" t="s">
         <v>286</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -5350,13 +5454,13 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
+      <c r="A90" s="5">
         <v>0</v>
       </c>
       <c r="B90" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" s="3" t="s">
         <v>289</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -5373,13 +5477,13 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="2">
+      <c r="A91" s="5">
         <v>0</v>
       </c>
       <c r="B91" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" s="3" t="s">
         <v>291</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -5396,13 +5500,13 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
+      <c r="A92" s="5">
         <v>0</v>
       </c>
       <c r="B92" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" s="3" t="s">
         <v>294</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -5419,13 +5523,13 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="2">
+      <c r="A93" s="5">
         <v>0</v>
       </c>
       <c r="B93" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" s="3" t="s">
         <v>297</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -5442,13 +5546,13 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="2">
+      <c r="A94" s="5">
         <v>0</v>
       </c>
       <c r="B94" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" s="3" t="s">
         <v>301</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -5465,13 +5569,13 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="2">
+      <c r="A95" s="5">
         <v>0</v>
       </c>
       <c r="B95" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" s="3" t="s">
         <v>305</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -5488,13 +5592,13 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="2">
+      <c r="A96" s="5">
         <v>0</v>
       </c>
       <c r="B96" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" s="3" t="s">
         <v>307</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -5511,13 +5615,13 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="2">
+      <c r="A97" s="5">
         <v>0</v>
       </c>
       <c r="B97" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C97" s="3" t="s">
         <v>310</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -5534,13 +5638,13 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="2">
+      <c r="A98" s="5">
         <v>0</v>
       </c>
       <c r="B98" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C98" s="3" t="s">
         <v>313</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -5557,13 +5661,13 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="2">
+      <c r="A99" s="5">
         <v>0</v>
       </c>
       <c r="B99" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" s="3" t="s">
         <v>317</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -5580,13 +5684,13 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="2">
+      <c r="A100" s="5">
         <v>0</v>
       </c>
       <c r="B100" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C100" s="3" t="s">
         <v>321</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -5603,13 +5707,13 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="2">
+      <c r="A101" s="5">
         <v>0</v>
       </c>
       <c r="B101" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" s="3" t="s">
         <v>324</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -5626,13 +5730,13 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="2">
+      <c r="A102" s="5">
         <v>0</v>
       </c>
       <c r="B102" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C102" s="3" t="s">
         <v>327</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -5649,13 +5753,13 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="2">
+      <c r="A103" s="5">
         <v>0</v>
       </c>
       <c r="B103" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" s="3" t="s">
         <v>330</v>
       </c>
       <c r="D103" s="1" t="s">
@@ -5672,13 +5776,13 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="2">
+      <c r="A104" s="5">
         <v>0</v>
       </c>
       <c r="B104" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="3" t="s">
         <v>333</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -5695,13 +5799,13 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="2">
+      <c r="A105" s="5">
         <v>0</v>
       </c>
       <c r="B105" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C105" s="3" t="s">
         <v>337</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -5718,13 +5822,13 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="2">
+      <c r="A106" s="5">
         <v>0</v>
       </c>
       <c r="B106" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="C106" s="3" t="s">
         <v>341</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -5741,13 +5845,13 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="2">
+      <c r="A107" s="5">
         <v>0</v>
       </c>
       <c r="B107" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C107" s="3" t="s">
         <v>345</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -5764,13 +5868,13 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="2">
+      <c r="A108" s="5">
         <v>0</v>
       </c>
       <c r="B108" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C108" s="3" t="s">
         <v>349</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -5787,13 +5891,13 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="2">
+      <c r="A109" s="5">
         <v>0</v>
       </c>
       <c r="B109" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C109" s="3" t="s">
         <v>352</v>
       </c>
       <c r="D109" s="1" t="s">
@@ -5810,13 +5914,13 @@
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="2">
+      <c r="A110" s="5">
         <v>0</v>
       </c>
       <c r="B110" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="C110" s="3" t="s">
         <v>355</v>
       </c>
       <c r="D110" s="1" t="s">
@@ -5833,13 +5937,13 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="2">
+      <c r="A111" s="5">
         <v>0</v>
       </c>
       <c r="B111" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C111" s="3" t="s">
         <v>359</v>
       </c>
       <c r="D111" s="1" t="s">
@@ -5856,13 +5960,13 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="2">
+      <c r="A112" s="5">
         <v>0</v>
       </c>
       <c r="B112" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C112" s="3" t="s">
         <v>362</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -5879,13 +5983,13 @@
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="2">
+      <c r="A113" s="5">
         <v>0</v>
       </c>
       <c r="B113" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C113" s="3" t="s">
         <v>366</v>
       </c>
       <c r="D113" s="1" t="s">
@@ -5902,13 +6006,13 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="2">
+      <c r="A114" s="5">
         <v>0</v>
       </c>
       <c r="B114" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C114" s="3" t="s">
         <v>369</v>
       </c>
       <c r="D114" s="1" t="s">
@@ -5925,13 +6029,13 @@
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="2">
+      <c r="A115" s="5">
         <v>0</v>
       </c>
       <c r="B115" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C115" s="3" t="s">
         <v>372</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -5948,13 +6052,13 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="2">
+      <c r="A116" s="5">
         <v>0</v>
       </c>
       <c r="B116" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C116" s="3" t="s">
         <v>376</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -5971,13 +6075,13 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="2">
+      <c r="A117" s="5">
         <v>0</v>
       </c>
       <c r="B117" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C117" s="3" t="s">
         <v>380</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -5994,13 +6098,13 @@
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="2">
+      <c r="A118" s="5">
         <v>0</v>
       </c>
       <c r="B118" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C118" s="3" t="s">
         <v>383</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -6017,13 +6121,13 @@
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="2">
+      <c r="A119" s="5">
         <v>0</v>
       </c>
       <c r="B119" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C119" s="3" t="s">
         <v>386</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -6040,13 +6144,13 @@
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="2">
+      <c r="A120" s="5">
         <v>0</v>
       </c>
       <c r="B120" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C120" s="3" t="s">
         <v>389</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -6063,13 +6167,13 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="2">
+      <c r="A121" s="5">
         <v>0</v>
       </c>
       <c r="B121" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="C121" s="3" t="s">
         <v>393</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -6086,13 +6190,13 @@
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="2">
+      <c r="A122" s="5">
         <v>0</v>
       </c>
       <c r="B122" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="C122" s="3" t="s">
         <v>396</v>
       </c>
       <c r="D122" s="1" t="s">
@@ -6109,13 +6213,13 @@
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A123" s="2">
+      <c r="A123" s="5">
         <v>0</v>
       </c>
       <c r="B123" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="C123" s="3" t="s">
         <v>399</v>
       </c>
       <c r="D123" s="1" t="s">
@@ -6132,13 +6236,13 @@
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" s="2">
+      <c r="A124" s="5">
         <v>0</v>
       </c>
       <c r="B124" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="C124" s="3" t="s">
         <v>403</v>
       </c>
       <c r="D124" s="1" t="s">
@@ -6155,13 +6259,13 @@
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A125" s="2">
+      <c r="A125" s="5">
         <v>0</v>
       </c>
       <c r="B125" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C125" s="3" t="s">
         <v>407</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -6178,13 +6282,13 @@
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A126" s="2">
+      <c r="A126" s="5">
         <v>0</v>
       </c>
       <c r="B126" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="C126" s="3" t="s">
         <v>410</v>
       </c>
       <c r="D126" s="1" t="s">
@@ -6201,13 +6305,13 @@
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" s="2">
+      <c r="A127" s="5">
         <v>0</v>
       </c>
       <c r="B127" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="C127" s="3" t="s">
         <v>413</v>
       </c>
       <c r="D127" s="1" t="s">
@@ -6224,13 +6328,13 @@
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A128" s="2">
+      <c r="A128" s="5">
         <v>0</v>
       </c>
       <c r="B128" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="C128" s="3" t="s">
         <v>416</v>
       </c>
       <c r="D128" s="1" t="s">
@@ -6247,13 +6351,13 @@
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A129" s="2">
+      <c r="A129" s="5">
         <v>0</v>
       </c>
       <c r="B129" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="C129" s="3" t="s">
         <v>420</v>
       </c>
       <c r="D129" s="1" t="s">
@@ -6270,13 +6374,13 @@
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" s="2">
+      <c r="A130" s="5">
         <v>0</v>
       </c>
       <c r="B130" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="C130" s="3" t="s">
         <v>424</v>
       </c>
       <c r="D130" s="1" t="s">
@@ -6293,13 +6397,13 @@
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A131" s="2">
+      <c r="A131" s="5">
         <v>0</v>
       </c>
       <c r="B131" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="C131" s="3" t="s">
         <v>427</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -6316,13 +6420,13 @@
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A132" s="2">
+      <c r="A132" s="5">
         <v>0</v>
       </c>
       <c r="B132" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C132" s="1" t="s">
+      <c r="C132" s="3" t="s">
         <v>430</v>
       </c>
       <c r="D132" s="1" t="s">
@@ -6339,13 +6443,13 @@
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A133" s="2">
+      <c r="A133" s="5">
         <v>0</v>
       </c>
       <c r="B133" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C133" s="1" t="s">
+      <c r="C133" s="3" t="s">
         <v>434</v>
       </c>
       <c r="D133" s="1" t="s">
@@ -6362,13 +6466,13 @@
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A134" s="2">
+      <c r="A134" s="5">
         <v>0</v>
       </c>
       <c r="B134" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="C134" s="3" t="s">
         <v>437</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -6385,13 +6489,13 @@
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A135" s="2">
+      <c r="A135" s="5">
         <v>0</v>
       </c>
       <c r="B135" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C135" s="1" t="s">
+      <c r="C135" s="3" t="s">
         <v>439</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -6408,13 +6512,13 @@
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A136" s="2">
+      <c r="A136" s="5">
         <v>0</v>
       </c>
       <c r="B136" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C136" s="1" t="s">
+      <c r="C136" s="3" t="s">
         <v>442</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -6431,13 +6535,13 @@
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A137" s="2">
+      <c r="A137" s="5">
         <v>0</v>
       </c>
       <c r="B137" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C137" s="1" t="s">
+      <c r="C137" s="3" t="s">
         <v>446</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -6454,13 +6558,13 @@
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" s="2">
+      <c r="A138" s="5">
         <v>0</v>
       </c>
       <c r="B138" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C138" s="1" t="s">
+      <c r="C138" s="3" t="s">
         <v>449</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -6477,13 +6581,13 @@
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A139" s="2">
+      <c r="A139" s="5">
         <v>0</v>
       </c>
       <c r="B139" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="C139" s="3" t="s">
         <v>453</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -6500,13 +6604,13 @@
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A140" s="2">
+      <c r="A140" s="5">
         <v>0</v>
       </c>
       <c r="B140" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C140" s="1" t="s">
+      <c r="C140" s="3" t="s">
         <v>457</v>
       </c>
       <c r="D140" s="1" t="s">
@@ -6523,13 +6627,13 @@
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A141" s="2">
+      <c r="A141" s="5">
         <v>0</v>
       </c>
       <c r="B141" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C141" s="1" t="s">
+      <c r="C141" s="3" t="s">
         <v>460</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -6546,13 +6650,13 @@
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A142" s="2">
+      <c r="A142" s="5">
         <v>0</v>
       </c>
       <c r="B142" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="C142" s="3" t="s">
         <v>464</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -6569,13 +6673,13 @@
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A143" s="2">
+      <c r="A143" s="5">
         <v>0</v>
       </c>
       <c r="B143" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C143" s="1" t="s">
+      <c r="C143" s="3" t="s">
         <v>467</v>
       </c>
       <c r="D143" s="1" t="s">
@@ -6592,13 +6696,13 @@
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A144" s="2">
+      <c r="A144" s="5">
         <v>0</v>
       </c>
       <c r="B144" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C144" s="1" t="s">
+      <c r="C144" s="3" t="s">
         <v>471</v>
       </c>
       <c r="D144" s="1" t="s">
@@ -6615,13 +6719,13 @@
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A145" s="2">
+      <c r="A145" s="5">
         <v>0</v>
       </c>
       <c r="B145" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C145" s="1" t="s">
+      <c r="C145" s="3" t="s">
         <v>474</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -6638,13 +6742,13 @@
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A146" s="2">
+      <c r="A146" s="5">
         <v>0</v>
       </c>
       <c r="B146" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="C146" s="3" t="s">
         <v>478</v>
       </c>
       <c r="D146" s="1" t="s">
@@ -6661,13 +6765,13 @@
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A147" s="2">
+      <c r="A147" s="5">
         <v>0</v>
       </c>
       <c r="B147" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C147" s="1" t="s">
+      <c r="C147" s="3" t="s">
         <v>481</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -6684,13 +6788,13 @@
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A148" s="2">
+      <c r="A148" s="5">
         <v>0</v>
       </c>
       <c r="B148" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C148" s="1" t="s">
+      <c r="C148" s="3" t="s">
         <v>484</v>
       </c>
       <c r="D148" s="1" t="s">
@@ -6707,13 +6811,13 @@
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A149" s="2">
+      <c r="A149" s="5">
         <v>0</v>
       </c>
       <c r="B149" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C149" s="1" t="s">
+      <c r="C149" s="3" t="s">
         <v>488</v>
       </c>
       <c r="D149" s="1" t="s">
@@ -6730,13 +6834,13 @@
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A150" s="2">
+      <c r="A150" s="5">
         <v>0</v>
       </c>
       <c r="B150" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C150" s="1" t="s">
+      <c r="C150" s="3" t="s">
         <v>491</v>
       </c>
       <c r="D150" s="1" t="s">
@@ -6753,13 +6857,13 @@
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A151" s="2">
+      <c r="A151" s="5">
         <v>0</v>
       </c>
       <c r="B151" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C151" s="1" t="s">
+      <c r="C151" s="3" t="s">
         <v>495</v>
       </c>
       <c r="D151" s="1" t="s">
@@ -6776,13 +6880,13 @@
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A152" s="2">
+      <c r="A152" s="5">
         <v>0</v>
       </c>
       <c r="B152" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C152" s="1" t="s">
+      <c r="C152" s="3" t="s">
         <v>498</v>
       </c>
       <c r="D152" s="1" t="s">
@@ -6799,13 +6903,13 @@
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A153" s="2">
+      <c r="A153" s="5">
         <v>0</v>
       </c>
       <c r="B153" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C153" s="1" t="s">
+      <c r="C153" s="3" t="s">
         <v>501</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -6822,13 +6926,13 @@
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A154" s="2">
+      <c r="A154" s="5">
         <v>0</v>
       </c>
       <c r="B154" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C154" s="1" t="s">
+      <c r="C154" s="3" t="s">
         <v>504</v>
       </c>
       <c r="D154" s="1" t="s">
@@ -6845,13 +6949,13 @@
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A155" s="2">
+      <c r="A155" s="5">
         <v>0</v>
       </c>
       <c r="B155" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C155" s="1" t="s">
+      <c r="C155" s="3" t="s">
         <v>507</v>
       </c>
       <c r="D155" s="1" t="s">
@@ -6868,13 +6972,13 @@
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A156" s="2">
+      <c r="A156" s="5">
         <v>0</v>
       </c>
       <c r="B156" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C156" s="1" t="s">
+      <c r="C156" s="3" t="s">
         <v>511</v>
       </c>
       <c r="D156" s="1" t="s">
@@ -6891,13 +6995,13 @@
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A157" s="2">
+      <c r="A157" s="5">
         <v>0</v>
       </c>
       <c r="B157" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C157" s="1" t="s">
+      <c r="C157" s="3" t="s">
         <v>515</v>
       </c>
       <c r="D157" s="1" t="s">
@@ -6914,13 +7018,13 @@
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A158" s="2">
+      <c r="A158" s="5">
         <v>0</v>
       </c>
       <c r="B158" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C158" s="1" t="s">
+      <c r="C158" s="3" t="s">
         <v>519</v>
       </c>
       <c r="D158" s="1" t="s">
@@ -6937,13 +7041,13 @@
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A159" s="2">
+      <c r="A159" s="5">
         <v>0</v>
       </c>
       <c r="B159" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C159" s="1" t="s">
+      <c r="C159" s="3" t="s">
         <v>522</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -6960,13 +7064,13 @@
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A160" s="2">
+      <c r="A160" s="5">
         <v>0</v>
       </c>
       <c r="B160" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C160" s="1" t="s">
+      <c r="C160" s="3" t="s">
         <v>525</v>
       </c>
       <c r="D160" s="1" t="s">
@@ -6983,13 +7087,13 @@
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A161" s="2">
+      <c r="A161" s="5">
         <v>0</v>
       </c>
       <c r="B161" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C161" s="1" t="s">
+      <c r="C161" s="3" t="s">
         <v>529</v>
       </c>
       <c r="D161" s="1" t="s">
@@ -7006,13 +7110,13 @@
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A162" s="2">
+      <c r="A162" s="5">
         <v>0</v>
       </c>
       <c r="B162" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C162" s="1" t="s">
+      <c r="C162" s="3" t="s">
         <v>532</v>
       </c>
       <c r="D162" s="1" t="s">
@@ -7029,13 +7133,13 @@
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A163" s="2">
+      <c r="A163" s="5">
         <v>0</v>
       </c>
       <c r="B163" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C163" s="1" t="s">
+      <c r="C163" s="3" t="s">
         <v>535</v>
       </c>
       <c r="D163" s="1" t="s">
@@ -7052,13 +7156,13 @@
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A164" s="2">
+      <c r="A164" s="5">
         <v>0</v>
       </c>
       <c r="B164" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C164" s="1" t="s">
+      <c r="C164" s="3" t="s">
         <v>538</v>
       </c>
       <c r="D164" s="1" t="s">
@@ -7075,13 +7179,13 @@
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A165" s="2">
+      <c r="A165" s="5">
         <v>0</v>
       </c>
       <c r="B165" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C165" s="1" t="s">
+      <c r="C165" s="3" t="s">
         <v>541</v>
       </c>
       <c r="D165" s="1" t="s">
@@ -7098,13 +7202,13 @@
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A166" s="2">
+      <c r="A166" s="5">
         <v>0</v>
       </c>
       <c r="B166" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C166" s="1" t="s">
+      <c r="C166" s="3" t="s">
         <v>544</v>
       </c>
       <c r="D166" s="1" t="s">
@@ -7121,13 +7225,13 @@
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A167" s="2">
+      <c r="A167" s="5">
         <v>0</v>
       </c>
       <c r="B167" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C167" s="1" t="s">
+      <c r="C167" s="3" t="s">
         <v>547</v>
       </c>
       <c r="D167" s="1" t="s">
@@ -7144,13 +7248,13 @@
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A168" s="2">
+      <c r="A168" s="5">
         <v>0</v>
       </c>
       <c r="B168" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C168" s="1" t="s">
+      <c r="C168" s="3" t="s">
         <v>551</v>
       </c>
       <c r="D168" s="1" t="s">
@@ -7167,13 +7271,13 @@
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A169" s="2">
+      <c r="A169" s="5">
         <v>0</v>
       </c>
       <c r="B169" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C169" s="1" t="s">
+      <c r="C169" s="3" t="s">
         <v>554</v>
       </c>
       <c r="D169" s="1" t="s">
@@ -7190,13 +7294,13 @@
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A170" s="2">
+      <c r="A170" s="5">
         <v>0</v>
       </c>
       <c r="B170" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C170" s="1" t="s">
+      <c r="C170" s="3" t="s">
         <v>557</v>
       </c>
       <c r="D170" s="1" t="s">
@@ -7213,13 +7317,13 @@
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A171" s="2">
+      <c r="A171" s="5">
         <v>0</v>
       </c>
       <c r="B171" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C171" s="1" t="s">
+      <c r="C171" s="3" t="s">
         <v>561</v>
       </c>
       <c r="D171" s="1" t="s">
@@ -7236,13 +7340,13 @@
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A172" s="2">
+      <c r="A172" s="5">
         <v>0</v>
       </c>
       <c r="B172" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C172" s="1" t="s">
+      <c r="C172" s="3" t="s">
         <v>564</v>
       </c>
       <c r="D172" s="1" t="s">
@@ -7259,13 +7363,13 @@
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A173" s="2">
+      <c r="A173" s="5">
         <v>0</v>
       </c>
       <c r="B173" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C173" s="1" t="s">
+      <c r="C173" s="3" t="s">
         <v>567</v>
       </c>
       <c r="D173" s="1" t="s">
@@ -7282,13 +7386,13 @@
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A174" s="2">
+      <c r="A174" s="5">
         <v>0</v>
       </c>
       <c r="B174" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C174" s="1" t="s">
+      <c r="C174" s="3" t="s">
         <v>570</v>
       </c>
       <c r="D174" s="1" t="s">
@@ -7305,13 +7409,13 @@
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A175" s="2">
+      <c r="A175" s="5">
         <v>0</v>
       </c>
       <c r="B175" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C175" s="1" t="s">
+      <c r="C175" s="3" t="s">
         <v>573</v>
       </c>
       <c r="D175" s="1" t="s">
@@ -7328,13 +7432,13 @@
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A176" s="2">
+      <c r="A176" s="5">
         <v>0</v>
       </c>
       <c r="B176" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C176" s="1" t="s">
+      <c r="C176" s="3" t="s">
         <v>577</v>
       </c>
       <c r="D176" s="1" t="s">
@@ -7351,13 +7455,13 @@
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A177" s="2">
+      <c r="A177" s="5">
         <v>0</v>
       </c>
       <c r="B177" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C177" s="1" t="s">
+      <c r="C177" s="3" t="s">
         <v>581</v>
       </c>
       <c r="D177" s="1" t="s">
@@ -7374,13 +7478,13 @@
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A178" s="2">
+      <c r="A178" s="5">
         <v>0</v>
       </c>
       <c r="B178" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C178" s="1" t="s">
+      <c r="C178" s="3" t="s">
         <v>585</v>
       </c>
       <c r="D178" s="1" t="s">
@@ -7397,13 +7501,13 @@
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A179" s="2">
+      <c r="A179" s="5">
         <v>0</v>
       </c>
       <c r="B179" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C179" s="1" t="s">
+      <c r="C179" s="3" t="s">
         <v>588</v>
       </c>
       <c r="D179" s="1" t="s">
@@ -7420,13 +7524,13 @@
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A180" s="2">
+      <c r="A180" s="5">
         <v>0</v>
       </c>
       <c r="B180" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C180" s="1" t="s">
+      <c r="C180" s="3" t="s">
         <v>591</v>
       </c>
       <c r="D180" s="1" t="s">
@@ -7443,13 +7547,13 @@
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A181" s="2">
+      <c r="A181" s="5">
         <v>0</v>
       </c>
       <c r="B181" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C181" s="1" t="s">
+      <c r="C181" s="3" t="s">
         <v>595</v>
       </c>
       <c r="D181" s="1" t="s">
@@ -7466,13 +7570,13 @@
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A182" s="2">
+      <c r="A182" s="5">
         <v>0</v>
       </c>
       <c r="B182" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C182" s="1" t="s">
+      <c r="C182" s="3" t="s">
         <v>599</v>
       </c>
       <c r="D182" s="1" t="s">
@@ -7489,13 +7593,13 @@
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A183" s="2">
+      <c r="A183" s="5">
         <v>0</v>
       </c>
       <c r="B183" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C183" s="1" t="s">
+      <c r="C183" s="3" t="s">
         <v>602</v>
       </c>
       <c r="D183" s="1" t="s">
@@ -7512,13 +7616,13 @@
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A184" s="2">
+      <c r="A184" s="5">
         <v>0</v>
       </c>
       <c r="B184" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C184" s="1" t="s">
+      <c r="C184" s="3" t="s">
         <v>605</v>
       </c>
       <c r="D184" s="1" t="s">
@@ -7535,13 +7639,13 @@
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A185" s="2">
+      <c r="A185" s="5">
         <v>0</v>
       </c>
       <c r="B185" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C185" s="1" t="s">
+      <c r="C185" s="3" t="s">
         <v>608</v>
       </c>
       <c r="D185" s="1" t="s">
@@ -7558,13 +7662,13 @@
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A186" s="2">
+      <c r="A186" s="5">
         <v>0</v>
       </c>
       <c r="B186" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C186" s="1" t="s">
+      <c r="C186" s="3" t="s">
         <v>611</v>
       </c>
       <c r="D186" s="1" t="s">
@@ -7581,13 +7685,13 @@
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A187" s="2">
+      <c r="A187" s="5">
         <v>0</v>
       </c>
       <c r="B187" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C187" s="1" t="s">
+      <c r="C187" s="3" t="s">
         <v>614</v>
       </c>
       <c r="D187" s="1" t="s">
@@ -7604,13 +7708,13 @@
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A188" s="2">
+      <c r="A188" s="5">
         <v>0</v>
       </c>
       <c r="B188" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C188" s="1" t="s">
+      <c r="C188" s="3" t="s">
         <v>617</v>
       </c>
       <c r="D188" s="1" t="s">
@@ -7627,13 +7731,13 @@
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A189" s="2">
+      <c r="A189" s="5">
         <v>0</v>
       </c>
       <c r="B189" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C189" s="1" t="s">
+      <c r="C189" s="3" t="s">
         <v>621</v>
       </c>
       <c r="D189" s="1" t="s">
@@ -7650,13 +7754,13 @@
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A190" s="2">
+      <c r="A190" s="5">
         <v>0</v>
       </c>
       <c r="B190" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C190" s="1" t="s">
+      <c r="C190" s="3" t="s">
         <v>624</v>
       </c>
       <c r="D190" s="1" t="s">
@@ -7673,13 +7777,13 @@
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A191" s="2">
+      <c r="A191" s="5">
         <v>0</v>
       </c>
       <c r="B191" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C191" s="1" t="s">
+      <c r="C191" s="3" t="s">
         <v>628</v>
       </c>
       <c r="D191" s="1" t="s">
@@ -7696,13 +7800,13 @@
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A192" s="2">
+      <c r="A192" s="5">
         <v>0</v>
       </c>
       <c r="B192" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C192" s="1" t="s">
+      <c r="C192" s="3" t="s">
         <v>631</v>
       </c>
       <c r="D192" s="1" t="s">
@@ -7719,13 +7823,13 @@
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A193" s="2">
+      <c r="A193" s="5">
         <v>0</v>
       </c>
       <c r="B193" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C193" s="1" t="s">
+      <c r="C193" s="3" t="s">
         <v>635</v>
       </c>
       <c r="D193" s="1" t="s">
@@ -7742,13 +7846,13 @@
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A194" s="2">
+      <c r="A194" s="5">
         <v>0</v>
       </c>
       <c r="B194" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C194" s="1" t="s">
+      <c r="C194" s="3" t="s">
         <v>638</v>
       </c>
       <c r="D194" s="1" t="s">
@@ -7765,13 +7869,13 @@
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A195" s="2">
+      <c r="A195" s="5">
         <v>0</v>
       </c>
       <c r="B195" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C195" s="1" t="s">
+      <c r="C195" s="3" t="s">
         <v>641</v>
       </c>
       <c r="D195" s="1" t="s">
@@ -7788,13 +7892,13 @@
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A196" s="2">
+      <c r="A196" s="5">
         <v>0</v>
       </c>
       <c r="B196" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C196" s="1" t="s">
+      <c r="C196" s="3" t="s">
         <v>644</v>
       </c>
       <c r="D196" s="1" t="s">
@@ -7811,13 +7915,13 @@
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A197" s="2">
+      <c r="A197" s="5">
         <v>0</v>
       </c>
       <c r="B197" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C197" s="1" t="s">
+      <c r="C197" s="3" t="s">
         <v>647</v>
       </c>
       <c r="D197" s="1" t="s">
@@ -7834,13 +7938,13 @@
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A198" s="2">
+      <c r="A198" s="5">
         <v>0</v>
       </c>
       <c r="B198" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C198" s="1" t="s">
+      <c r="C198" s="3" t="s">
         <v>650</v>
       </c>
       <c r="D198" s="1" t="s">
@@ -7857,13 +7961,13 @@
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A199" s="2">
+      <c r="A199" s="5">
         <v>0</v>
       </c>
       <c r="B199" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C199" s="1" t="s">
+      <c r="C199" s="3" t="s">
         <v>653</v>
       </c>
       <c r="D199" s="1" t="s">
@@ -7880,13 +7984,13 @@
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A200" s="2">
+      <c r="A200" s="5">
         <v>0</v>
       </c>
       <c r="B200" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C200" s="1" t="s">
+      <c r="C200" s="3" t="s">
         <v>657</v>
       </c>
       <c r="D200" s="1" t="s">
@@ -7903,13 +8007,13 @@
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A201" s="2">
+      <c r="A201" s="5">
         <v>0</v>
       </c>
       <c r="B201" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C201" s="1" t="s">
+      <c r="C201" s="3" t="s">
         <v>660</v>
       </c>
       <c r="D201" s="1" t="s">
@@ -7926,13 +8030,13 @@
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A202" s="2">
+      <c r="A202" s="5">
         <v>0</v>
       </c>
       <c r="B202" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C202" s="1" t="s">
+      <c r="C202" s="3" t="s">
         <v>664</v>
       </c>
       <c r="D202" s="1" t="s">
@@ -7949,13 +8053,13 @@
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A203" s="2">
+      <c r="A203" s="5">
         <v>0</v>
       </c>
       <c r="B203" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C203" s="1" t="s">
+      <c r="C203" s="3" t="s">
         <v>667</v>
       </c>
       <c r="D203" s="1" t="s">
@@ -7972,13 +8076,13 @@
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A204" s="2">
+      <c r="A204" s="5">
         <v>0</v>
       </c>
       <c r="B204" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C204" s="1" t="s">
+      <c r="C204" s="3" t="s">
         <v>670</v>
       </c>
       <c r="D204" s="1" t="s">
@@ -7995,13 +8099,13 @@
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A205" s="2">
+      <c r="A205" s="5">
         <v>0</v>
       </c>
       <c r="B205" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C205" s="1" t="s">
+      <c r="C205" s="3" t="s">
         <v>674</v>
       </c>
       <c r="D205" s="1" t="s">
@@ -8018,13 +8122,13 @@
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A206" s="2">
+      <c r="A206" s="5">
         <v>0</v>
       </c>
       <c r="B206" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C206" s="1" t="s">
+      <c r="C206" s="3" t="s">
         <v>677</v>
       </c>
       <c r="D206" s="1" t="s">
@@ -8041,13 +8145,13 @@
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A207" s="2">
+      <c r="A207" s="5">
         <v>0</v>
       </c>
       <c r="B207" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C207" s="1" t="s">
+      <c r="C207" s="3" t="s">
         <v>681</v>
       </c>
       <c r="D207" s="1" t="s">
@@ -8064,13 +8168,13 @@
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A208" s="2">
+      <c r="A208" s="5">
         <v>0</v>
       </c>
       <c r="B208" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C208" s="1" t="s">
+      <c r="C208" s="3" t="s">
         <v>684</v>
       </c>
       <c r="D208" s="1" t="s">
@@ -8087,13 +8191,13 @@
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A209" s="2">
+      <c r="A209" s="5">
         <v>0</v>
       </c>
       <c r="B209" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C209" s="1" t="s">
+      <c r="C209" s="3" t="s">
         <v>687</v>
       </c>
       <c r="D209" s="1" t="s">
@@ -8110,13 +8214,13 @@
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A210" s="2">
+      <c r="A210" s="5">
         <v>0</v>
       </c>
       <c r="B210" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C210" s="1" t="s">
+      <c r="C210" s="3" t="s">
         <v>690</v>
       </c>
       <c r="D210" s="1" t="s">
@@ -8133,13 +8237,13 @@
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A211" s="2">
+      <c r="A211" s="5">
         <v>0</v>
       </c>
       <c r="B211" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C211" s="1" t="s">
+      <c r="C211" s="3" t="s">
         <v>693</v>
       </c>
       <c r="D211" s="1" t="s">
@@ -8156,13 +8260,13 @@
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A212" s="2">
+      <c r="A212" s="5">
         <v>0</v>
       </c>
       <c r="B212" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C212" s="1" t="s">
+      <c r="C212" s="3" t="s">
         <v>697</v>
       </c>
       <c r="D212" s="1" t="s">
@@ -8179,13 +8283,13 @@
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A213" s="2">
+      <c r="A213" s="5">
         <v>0</v>
       </c>
       <c r="B213" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C213" s="1" t="s">
+      <c r="C213" s="3" t="s">
         <v>700</v>
       </c>
       <c r="D213" s="1" t="s">
@@ -8202,13 +8306,13 @@
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A214" s="2">
+      <c r="A214" s="5">
         <v>0</v>
       </c>
       <c r="B214" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C214" s="1" t="s">
+      <c r="C214" s="3" t="s">
         <v>703</v>
       </c>
       <c r="D214" s="1" t="s">
@@ -8225,13 +8329,13 @@
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A215" s="2">
+      <c r="A215" s="5">
         <v>0</v>
       </c>
       <c r="B215" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C215" s="1" t="s">
+      <c r="C215" s="3" t="s">
         <v>707</v>
       </c>
       <c r="D215" s="1" t="s">
@@ -8248,13 +8352,13 @@
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A216" s="2">
+      <c r="A216" s="5">
         <v>0</v>
       </c>
       <c r="B216" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C216" s="1" t="s">
+      <c r="C216" s="3" t="s">
         <v>711</v>
       </c>
       <c r="D216" s="1" t="s">
@@ -8271,13 +8375,13 @@
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A217" s="2">
+      <c r="A217" s="5">
         <v>0</v>
       </c>
       <c r="B217" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C217" s="1" t="s">
+      <c r="C217" s="3" t="s">
         <v>714</v>
       </c>
       <c r="D217" s="1" t="s">
@@ -8294,13 +8398,13 @@
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A218" s="2">
+      <c r="A218" s="5">
         <v>0</v>
       </c>
       <c r="B218" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C218" s="1" t="s">
+      <c r="C218" s="3" t="s">
         <v>717</v>
       </c>
       <c r="D218" s="1" t="s">
@@ -8317,13 +8421,13 @@
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A219" s="2">
+      <c r="A219" s="5">
         <v>0</v>
       </c>
       <c r="B219" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C219" s="1" t="s">
+      <c r="C219" s="3" t="s">
         <v>720</v>
       </c>
       <c r="D219" s="1" t="s">
@@ -8340,13 +8444,13 @@
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A220" s="2">
+      <c r="A220" s="5">
         <v>0</v>
       </c>
       <c r="B220" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C220" s="1" t="s">
+      <c r="C220" s="3" t="s">
         <v>723</v>
       </c>
       <c r="D220" s="1" t="s">
@@ -8363,13 +8467,13 @@
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A221" s="2">
+      <c r="A221" s="5">
         <v>0</v>
       </c>
       <c r="B221" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C221" s="1" t="s">
+      <c r="C221" s="3" t="s">
         <v>726</v>
       </c>
       <c r="D221" s="1" t="s">
@@ -8386,13 +8490,13 @@
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A222" s="2">
+      <c r="A222" s="5">
         <v>0</v>
       </c>
       <c r="B222" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C222" s="1" t="s">
+      <c r="C222" s="3" t="s">
         <v>731</v>
       </c>
       <c r="D222" s="1" t="s">
@@ -8409,13 +8513,13 @@
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A223" s="2">
+      <c r="A223" s="5">
         <v>0</v>
       </c>
       <c r="B223" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C223" s="1" t="s">
+      <c r="C223" s="3" t="s">
         <v>735</v>
       </c>
       <c r="D223" s="1" t="s">
@@ -8432,13 +8536,13 @@
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A224" s="2">
+      <c r="A224" s="5">
         <v>0</v>
       </c>
       <c r="B224" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C224" s="1" t="s">
+      <c r="C224" s="3" t="s">
         <v>739</v>
       </c>
       <c r="D224" s="1" t="s">
@@ -8455,13 +8559,13 @@
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A225" s="2">
+      <c r="A225" s="5">
         <v>0</v>
       </c>
       <c r="B225" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C225" s="1" t="s">
+      <c r="C225" s="3" t="s">
         <v>742</v>
       </c>
       <c r="D225" s="1" t="s">
@@ -8478,13 +8582,13 @@
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A226" s="2">
+      <c r="A226" s="5">
         <v>0</v>
       </c>
       <c r="B226" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C226" s="1" t="s">
+      <c r="C226" s="3" t="s">
         <v>745</v>
       </c>
       <c r="D226" s="1" t="s">
@@ -8501,13 +8605,13 @@
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A227" s="2">
+      <c r="A227" s="5">
         <v>0</v>
       </c>
       <c r="B227" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C227" s="1" t="s">
+      <c r="C227" s="3" t="s">
         <v>748</v>
       </c>
       <c r="D227" s="1" t="s">
@@ -8524,13 +8628,13 @@
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A228" s="2">
+      <c r="A228" s="5">
         <v>0</v>
       </c>
       <c r="B228" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C228" s="1" t="s">
+      <c r="C228" s="3" t="s">
         <v>751</v>
       </c>
       <c r="D228" s="1" t="s">
@@ -8547,13 +8651,13 @@
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A229" s="2">
+      <c r="A229" s="5">
         <v>0</v>
       </c>
       <c r="B229" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C229" s="1" t="s">
+      <c r="C229" s="3" t="s">
         <v>755</v>
       </c>
       <c r="D229" s="1" t="s">
@@ -8570,13 +8674,13 @@
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A230" s="2">
+      <c r="A230" s="5">
         <v>0</v>
       </c>
       <c r="B230" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C230" s="1" t="s">
+      <c r="C230" s="3" t="s">
         <v>759</v>
       </c>
       <c r="D230" s="1" t="s">
@@ -8593,13 +8697,13 @@
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A231" s="2">
+      <c r="A231" s="5">
         <v>0</v>
       </c>
       <c r="B231" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C231" s="1" t="s">
+      <c r="C231" s="3" t="s">
         <v>762</v>
       </c>
       <c r="D231" s="1" t="s">
@@ -8616,13 +8720,13 @@
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A232" s="2">
+      <c r="A232" s="5">
         <v>0</v>
       </c>
       <c r="B232" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C232" s="1" t="s">
+      <c r="C232" s="3" t="s">
         <v>766</v>
       </c>
       <c r="D232" s="1" t="s">
@@ -8639,13 +8743,13 @@
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A233" s="2">
+      <c r="A233" s="5">
         <v>0</v>
       </c>
       <c r="B233" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C233" s="1" t="s">
+      <c r="C233" s="3" t="s">
         <v>769</v>
       </c>
       <c r="D233" s="1" t="s">
@@ -8662,13 +8766,13 @@
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A234" s="2">
+      <c r="A234" s="5">
         <v>0</v>
       </c>
       <c r="B234" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C234" s="1" t="s">
+      <c r="C234" s="3" t="s">
         <v>772</v>
       </c>
       <c r="D234" s="1" t="s">
@@ -8685,13 +8789,13 @@
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A235" s="2">
+      <c r="A235" s="5">
         <v>0</v>
       </c>
       <c r="B235" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C235" s="1" t="s">
+      <c r="C235" s="3" t="s">
         <v>775</v>
       </c>
       <c r="D235" s="1" t="s">
@@ -8708,13 +8812,13 @@
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A236" s="2">
+      <c r="A236" s="5">
         <v>0</v>
       </c>
       <c r="B236" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C236" s="1" t="s">
+      <c r="C236" s="3" t="s">
         <v>778</v>
       </c>
       <c r="D236" s="1" t="s">
@@ -8731,13 +8835,13 @@
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A237" s="2">
+      <c r="A237" s="5">
         <v>0</v>
       </c>
       <c r="B237" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C237" s="1" t="s">
+      <c r="C237" s="3" t="s">
         <v>781</v>
       </c>
       <c r="D237" s="1" t="s">
@@ -8754,13 +8858,13 @@
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A238" s="2">
+      <c r="A238" s="5">
         <v>0</v>
       </c>
       <c r="B238" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C238" s="1" t="s">
+      <c r="C238" s="3" t="s">
         <v>781</v>
       </c>
       <c r="D238" s="1" t="s">
@@ -8777,13 +8881,13 @@
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A239" s="2">
+      <c r="A239" s="5">
         <v>0</v>
       </c>
       <c r="B239" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C239" s="1" t="s">
+      <c r="C239" s="3" t="s">
         <v>786</v>
       </c>
       <c r="D239" s="1" t="s">
@@ -8800,13 +8904,13 @@
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A240" s="2">
+      <c r="A240" s="5">
         <v>0</v>
       </c>
       <c r="B240" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C240" s="1" t="s">
+      <c r="C240" s="3" t="s">
         <v>739</v>
       </c>
       <c r="D240" s="1" t="s">
@@ -8819,6 +8923,832 @@
         <v>790</v>
       </c>
       <c r="G240" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A241" s="5">
+        <v>0</v>
+      </c>
+      <c r="B241" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C241" s="3">
+        <v>257</v>
+      </c>
+      <c r="D241" s="1">
+        <v>14011502910</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="F241" s="1">
+        <v>14011502910</v>
+      </c>
+      <c r="G241" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A242" s="5">
+        <v>0</v>
+      </c>
+      <c r="B242" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C242" s="3">
+        <v>258</v>
+      </c>
+      <c r="D242" s="1">
+        <v>411445863143</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="F242" s="1">
+        <v>10260701249</v>
+      </c>
+      <c r="G242" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A243" s="5">
+        <v>0</v>
+      </c>
+      <c r="B243" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C243" s="3">
+        <v>259</v>
+      </c>
+      <c r="D243" s="1">
+        <v>10380098441</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="F243" s="1">
+        <v>10380098441</v>
+      </c>
+      <c r="G243" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A244" s="5">
+        <v>0</v>
+      </c>
+      <c r="B244" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C244" s="3">
+        <v>260</v>
+      </c>
+      <c r="D244" s="1">
+        <v>14007633920</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="F244" s="1">
+        <v>14007633920</v>
+      </c>
+      <c r="G244" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A245" s="5">
+        <v>0</v>
+      </c>
+      <c r="B245" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C245" s="3">
+        <v>261</v>
+      </c>
+      <c r="D245" s="1">
+        <v>14007180670</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="F245" s="1">
+        <v>14007180670</v>
+      </c>
+      <c r="G245" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A246" s="5">
+        <v>0</v>
+      </c>
+      <c r="B246" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C246" s="3">
+        <v>262</v>
+      </c>
+      <c r="D246" s="1">
+        <v>14005386170</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="F246" s="1">
+        <v>14005386170</v>
+      </c>
+      <c r="G246" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A247" s="5">
+        <v>0</v>
+      </c>
+      <c r="B247" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C247" s="3">
+        <v>263</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="F247" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G247" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A248" s="5">
+        <v>0</v>
+      </c>
+      <c r="B248" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C248" s="3">
+        <v>264</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="F248" s="1">
+        <v>1199395412</v>
+      </c>
+      <c r="G248" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A249" s="5">
+        <v>0</v>
+      </c>
+      <c r="B249" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C249" s="3">
+        <v>265</v>
+      </c>
+      <c r="D249" s="1">
+        <v>411478649836</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="F249" s="1">
+        <v>14004723800</v>
+      </c>
+      <c r="G249" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A250" s="5">
+        <v>0</v>
+      </c>
+      <c r="B250" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C250" s="3">
+        <v>266</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E250" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="F250" s="1">
+        <v>1200185897</v>
+      </c>
+      <c r="G250" s="1">
+        <v>9162346845</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A251" s="5">
+        <v>0</v>
+      </c>
+      <c r="B251" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C251" s="3">
+        <v>267</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="F251" s="1">
+        <v>5120037283</v>
+      </c>
+      <c r="G251" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A252" s="5">
+        <v>0</v>
+      </c>
+      <c r="B252" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C252" s="3">
+        <v>268</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="F252" s="1">
+        <v>4623552675</v>
+      </c>
+      <c r="G252" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A253" s="5">
+        <v>0</v>
+      </c>
+      <c r="B253" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C253" s="3">
+        <v>269</v>
+      </c>
+      <c r="D253" s="1">
+        <v>10861767939</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="F253" s="1">
+        <v>10861767939</v>
+      </c>
+      <c r="G253" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A254" s="5">
+        <v>0</v>
+      </c>
+      <c r="B254" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C254" s="3">
+        <v>270</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="F254" s="1">
+        <v>5129840194</v>
+      </c>
+      <c r="G254" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A255" s="5">
+        <v>0</v>
+      </c>
+      <c r="B255" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C255" s="3">
+        <v>271</v>
+      </c>
+      <c r="D255" s="1">
+        <v>10260133548</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="F255" s="1">
+        <v>10260133548</v>
+      </c>
+      <c r="G255" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A256" s="5">
+        <v>0</v>
+      </c>
+      <c r="B256" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C256" s="3">
+        <v>272</v>
+      </c>
+      <c r="D256" s="1">
+        <v>14004289492</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="F256" s="1">
+        <v>14004289492</v>
+      </c>
+      <c r="G256" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A257" s="5">
+        <v>0</v>
+      </c>
+      <c r="B257" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C257" s="3">
+        <v>273</v>
+      </c>
+      <c r="D257" s="1">
+        <v>14010656216</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="F257" s="1">
+        <v>14010656216</v>
+      </c>
+      <c r="G257" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A258" s="5">
+        <v>0</v>
+      </c>
+      <c r="B258" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C258" s="3">
+        <v>274</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E258" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="F258" s="1">
+        <v>1190171732</v>
+      </c>
+      <c r="G258" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A259" s="5">
+        <v>0</v>
+      </c>
+      <c r="B259" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C259" s="3">
+        <v>275</v>
+      </c>
+      <c r="D259" s="1">
+        <v>10101874688</v>
+      </c>
+      <c r="E259" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="F259" s="1">
+        <v>10101874688</v>
+      </c>
+      <c r="G259" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A260" s="5">
+        <v>0</v>
+      </c>
+      <c r="B260" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C260" s="3">
+        <v>276</v>
+      </c>
+      <c r="D260" s="1">
+        <v>10720135832</v>
+      </c>
+      <c r="E260" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="F260" s="1">
+        <v>10720135832</v>
+      </c>
+      <c r="G260" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A261" s="5">
+        <v>0</v>
+      </c>
+      <c r="B261" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C261" s="3">
+        <v>277</v>
+      </c>
+      <c r="D261" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="F261" s="1">
+        <v>1200138740</v>
+      </c>
+      <c r="G261" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A262" s="5">
+        <v>0</v>
+      </c>
+      <c r="B262" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C262" s="3">
+        <v>278</v>
+      </c>
+      <c r="D262" s="1">
+        <v>14009154174</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="F262" s="1">
+        <v>14009154174</v>
+      </c>
+      <c r="G262" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A263" s="5">
+        <v>0</v>
+      </c>
+      <c r="B263" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C263" s="3">
+        <v>279</v>
+      </c>
+      <c r="D263" s="1">
+        <v>10101613123</v>
+      </c>
+      <c r="E263" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="F263" s="1">
+        <v>10101613123</v>
+      </c>
+      <c r="G263" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A264" s="5">
+        <v>0</v>
+      </c>
+      <c r="B264" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C264" s="3">
+        <v>280</v>
+      </c>
+      <c r="D264" s="1">
+        <v>10100302746</v>
+      </c>
+      <c r="E264" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="F264" s="1">
+        <v>10100302746</v>
+      </c>
+      <c r="G264" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A265" s="5">
+        <v>0</v>
+      </c>
+      <c r="B265" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C265" s="3">
+        <v>281</v>
+      </c>
+      <c r="D265" s="1">
+        <v>14005833221</v>
+      </c>
+      <c r="E265" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="F265" s="1">
+        <v>14005833221</v>
+      </c>
+      <c r="G265" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A266" s="5">
+        <v>0</v>
+      </c>
+      <c r="B266" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C266" s="3">
+        <v>282</v>
+      </c>
+      <c r="D266" s="1">
+        <v>10102764298</v>
+      </c>
+      <c r="E266" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="F266" s="1">
+        <v>10102764298</v>
+      </c>
+      <c r="G266" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A267" s="5">
+        <v>0</v>
+      </c>
+      <c r="B267" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C267" s="3">
+        <v>283</v>
+      </c>
+      <c r="D267" s="1">
+        <v>10260614050</v>
+      </c>
+      <c r="E267" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="F267" s="1">
+        <v>10260614050</v>
+      </c>
+      <c r="G267" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A268" s="5">
+        <v>0</v>
+      </c>
+      <c r="B268" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C268" s="3">
+        <v>284</v>
+      </c>
+      <c r="D268" s="1">
+        <v>10320531524</v>
+      </c>
+      <c r="E268" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="F268" s="1">
+        <v>10320531524</v>
+      </c>
+      <c r="G268" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A269" s="5">
+        <v>0</v>
+      </c>
+      <c r="B269" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C269" s="3">
+        <v>285</v>
+      </c>
+      <c r="D269" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E269" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="F269" s="1">
+        <v>2440116734</v>
+      </c>
+      <c r="G269" s="1">
+        <v>9928883454</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A270" s="5">
+        <v>0</v>
+      </c>
+      <c r="B270" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C270" s="3">
+        <v>286</v>
+      </c>
+      <c r="D270" s="1">
+        <v>10102639989</v>
+      </c>
+      <c r="E270" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="F270" s="1">
+        <v>10102639989</v>
+      </c>
+      <c r="G270" s="1"/>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A271" s="5">
+        <v>0</v>
+      </c>
+      <c r="B271" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C271" s="3">
+        <v>287</v>
+      </c>
+      <c r="D271" s="1">
+        <v>10801277810001</v>
+      </c>
+      <c r="E271" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="F271" s="1">
+        <v>1080127781</v>
+      </c>
+      <c r="G271" s="1">
+        <v>9137880584</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A272" s="5">
+        <v>0</v>
+      </c>
+      <c r="B272" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C272" s="3">
+        <v>288</v>
+      </c>
+      <c r="D272" s="1">
+        <v>11998100710001</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="F272" s="1">
+        <v>1199810071</v>
+      </c>
+      <c r="G272" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A273" s="5">
+        <v>0</v>
+      </c>
+      <c r="B273" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C273" s="3">
+        <v>289</v>
+      </c>
+      <c r="D273" s="1">
+        <v>14008747992</v>
+      </c>
+      <c r="E273" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="F273" s="1">
+        <v>14008747992</v>
+      </c>
+      <c r="G273" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A274" s="5">
+        <v>0</v>
+      </c>
+      <c r="B274" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C274" s="3">
+        <v>290</v>
+      </c>
+      <c r="D274" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E274" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="F274" s="1">
+        <v>50924321</v>
+      </c>
+      <c r="G274" s="1">
+        <v>9929397415</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A275" s="5">
+        <v>0</v>
+      </c>
+      <c r="B275" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C275" s="3">
+        <v>291</v>
+      </c>
+      <c r="D275" s="1">
+        <v>411397577914</v>
+      </c>
+      <c r="E275" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="F275" s="1">
+        <v>10420232190</v>
+      </c>
+      <c r="G275" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A276" s="5">
+        <v>0</v>
+      </c>
+      <c r="B276" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C276" s="3">
+        <v>292</v>
+      </c>
+      <c r="D276" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E276" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="F276" s="1">
+        <v>1190255431</v>
+      </c>
+      <c r="G276" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>